<commit_message>
excel read text black
</commit_message>
<xml_diff>
--- a/public/mydata/motion_control_system_requirements.xlsx
+++ b/public/mydata/motion_control_system_requirements.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SingurK\Documents\Data\Personal\AI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SingurK\Documents\Data\Personal\Apps\git_repo\Kausi-hub.github.io\public\mydata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF1FE195-5916-4E4F-8125-3191CE865736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67A50F0A-830F-4677-9DD5-ECC73FBCF861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1308" yWindow="1644" windowWidth="17280" windowHeight="10044" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="System Requirements" sheetId="1" r:id="rId1"/>
@@ -994,7 +994,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1025,6 +1025,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1307,8 +1310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:C39"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:XFD36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1318,9 +1321,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:3" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="12" t="s">
         <v>259</v>
       </c>
+      <c r="C1" s="12"/>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
@@ -1610,6 +1614,9 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1618,8 +1625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2B9BF03-FD0F-446C-85E8-96515BDB6AF4}">
   <dimension ref="B1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1629,9 +1636,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="12" t="s">
         <v>252</v>
       </c>
+      <c r="C1" s="12"/>
     </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
@@ -1765,9 +1773,10 @@
       </c>
     </row>
     <row r="13" spans="2:5" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="12" t="s">
         <v>253</v>
       </c>
+      <c r="C13" s="12"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
@@ -1882,6 +1891,10 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B13:C13"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1891,7 +1904,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2144,8 +2157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80DF5DD9-6A22-4413-A368-BED35DF2C99E}">
   <dimension ref="B1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2158,9 +2171,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="12" t="s">
         <v>255</v>
       </c>
+      <c r="C1" s="12"/>
     </row>
     <row r="2" spans="2:7" ht="18" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
@@ -2457,6 +2471,9 @@
       <c r="B38" s="7"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
excel merged cell rendering
</commit_message>
<xml_diff>
--- a/public/mydata/motion_control_system_requirements.xlsx
+++ b/public/mydata/motion_control_system_requirements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SingurK\Documents\Data\Personal\Apps\git_repo\Kausi-hub.github.io\public\mydata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046FA546-3AA2-4F27-BEBA-0C3A657DA75F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FEEA351-28AA-41D9-9DE3-DBFA63AFB037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1308" yWindow="1644" windowWidth="17280" windowHeight="10044" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,9 +31,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="265">
   <si>
-    <t>1. Functional Requirements</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
@@ -76,9 +73,6 @@
     <t>The control system shall support multiple drive modes (e.g., normal, sport, eco, autonomous).</t>
   </si>
   <si>
-    <t>2. Performance Requirements</t>
-  </si>
-  <si>
     <t>P.1</t>
   </si>
   <si>
@@ -115,9 +109,6 @@
     <t>The system shall operate reliably at vehicle speeds from 0 to 130 km/h.</t>
   </si>
   <si>
-    <t>3. Safety and Fault Tolerance Requirements</t>
-  </si>
-  <si>
     <t>S.1</t>
   </si>
   <si>
@@ -154,9 +145,6 @@
     <t>The system shall perform periodic self-tests on power-up and during operation.</t>
   </si>
   <si>
-    <t>4. Interface Requirements</t>
-  </si>
-  <si>
     <t>I.1</t>
   </si>
   <si>
@@ -181,9 +169,6 @@
     <t>Diagnostic and calibration interfaces shall be accessible via secure OBD-II or Ethernet ports.</t>
   </si>
   <si>
-    <t>5. Environmental &amp; Reliability Requirements</t>
-  </si>
-  <si>
     <t>E.1</t>
   </si>
   <si>
@@ -206,9 +191,6 @@
   </si>
   <si>
     <t>MTBF (Mean Time Between Failures) of the motion control actuation system shall exceed 10,000 hours.</t>
-  </si>
-  <si>
-    <t>6. Cybersecurity Requirements</t>
   </si>
   <si>
     <t>C.1</t>
@@ -909,12 +891,30 @@
   <si>
     <t xml:space="preserve">System Safety Concept </t>
   </si>
+  <si>
+    <t>Functional Requirements</t>
+  </si>
+  <si>
+    <t>Performance Requirements</t>
+  </si>
+  <si>
+    <t>Safety and Fault Tolerance Requirements</t>
+  </si>
+  <si>
+    <t>Interface Requirements</t>
+  </si>
+  <si>
+    <t>Environmental &amp; Reliability Requirements</t>
+  </si>
+  <si>
+    <t>Cybersecurity Requirements</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -962,6 +962,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -983,7 +991,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1014,17 +1022,20 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1308,8 +1319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1318,301 +1329,314 @@
     <col min="3" max="3" width="108.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="B1" s="12"/>
-      <c r="C1" s="13" t="s">
-        <v>251</v>
-      </c>
+    <row r="1" spans="2:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="C1" s="13"/>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="3" spans="2:3" ht="18" x14ac:dyDescent="0.3">
-      <c r="B3" s="2"/>
-      <c r="C3" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="B3" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="C3" s="14"/>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>3</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="10" spans="2:3" ht="18" x14ac:dyDescent="0.3">
-      <c r="C10" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="B10" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="C10" s="14"/>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B11" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B12" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B13" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B14" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B15" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B16" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="18" x14ac:dyDescent="0.3">
-      <c r="C17" s="2" t="s">
-        <v>28</v>
-      </c>
+      <c r="B17" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="C17" s="14"/>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B19" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B20" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B21" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B22" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B23" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="2:3" ht="18" x14ac:dyDescent="0.3">
-      <c r="C24" s="2" t="s">
-        <v>41</v>
-      </c>
+      <c r="B24" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="C24" s="14"/>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B25" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B26" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B27" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B28" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="2:3" ht="18" x14ac:dyDescent="0.3">
-      <c r="B29" s="2"/>
-      <c r="C29" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="B29" s="14" t="s">
+        <v>263</v>
+      </c>
+      <c r="C29" s="14"/>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B30" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>1</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B31" s="4" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B32" s="4" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B33" s="4" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B34" s="4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" spans="2:3" ht="18" x14ac:dyDescent="0.3">
-      <c r="C35" s="2" t="s">
-        <v>59</v>
-      </c>
+      <c r="B35" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="C35" s="14"/>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B36" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>1</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B37" s="4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B38" s="4" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B39" s="4" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B29:C29"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1621,8 +1645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2B9BF03-FD0F-446C-85E8-96515BDB6AF4}">
   <dimension ref="B1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1632,261 +1656,267 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="C1" s="15" t="s">
-        <v>248</v>
-      </c>
-      <c r="D1" s="15"/>
+      <c r="B1" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="C1" s="15"/>
+      <c r="D1" s="12"/>
     </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B10" s="4" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B11" s="4" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="C13" s="15" t="s">
-        <v>249</v>
-      </c>
+      <c r="B13" s="15" t="s">
+        <v>243</v>
+      </c>
+      <c r="C13" s="15"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B15" s="4" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B16" s="4" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="4" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B20" s="4" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="4" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B13:C13"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1896,7 +1926,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1906,240 +1936,256 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.3">
-      <c r="B1" s="14" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.3">
-      <c r="B2" s="2" t="s">
-        <v>200</v>
-      </c>
+      <c r="A1" s="13" t="s">
+        <v>241</v>
+      </c>
+      <c r="B1" s="13"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="B2" s="16"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="C4" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="D4" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C5" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="D5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="18" x14ac:dyDescent="0.3">
-      <c r="B6" s="2" t="s">
-        <v>203</v>
-      </c>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="B6" s="16"/>
     </row>
     <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="C7" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="D7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="C8" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="D8" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="18" x14ac:dyDescent="0.3">
-      <c r="B9" s="2" t="s">
-        <v>206</v>
-      </c>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="B9" s="16"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C10" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="D10" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="C11" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="D11" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="C12" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="D12" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="18" x14ac:dyDescent="0.3">
-      <c r="B13" s="2" t="s">
-        <v>210</v>
-      </c>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="B13" s="16"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C14" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="D14" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C15" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="D15" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="18" x14ac:dyDescent="0.3">
-      <c r="B16" s="2" t="s">
-        <v>212</v>
-      </c>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="B16" s="16"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="C17" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="D17" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="C18" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="D18" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="18" x14ac:dyDescent="0.3">
-      <c r="B19" s="2" t="s">
-        <v>215</v>
-      </c>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="B19" s="16"/>
     </row>
     <row r="20" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="C20" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="D20" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="C21" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="D21" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B22" s="6"/>
     </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A16:B16"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2150,7 +2196,7 @@
   <dimension ref="B1:G37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B17" sqref="B17:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2163,283 +2209,287 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="18" x14ac:dyDescent="0.3">
-      <c r="C1" s="15" t="s">
-        <v>264</v>
-      </c>
-      <c r="D1" s="15"/>
-    </row>
-    <row r="2" spans="2:7" ht="18" x14ac:dyDescent="0.3">
-      <c r="C2" s="2" t="s">
-        <v>261</v>
-      </c>
+      <c r="B1" s="15" t="s">
+        <v>258</v>
+      </c>
+      <c r="C1" s="15"/>
+      <c r="D1" s="12"/>
+    </row>
+    <row r="2" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B2" s="16" t="s">
+        <v>255</v>
+      </c>
+      <c r="C2" s="16"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="C3" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="C4" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="C5" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C7" s="8" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C8" s="8" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" ht="18" x14ac:dyDescent="0.3">
-      <c r="C9" s="2" t="s">
-        <v>262</v>
-      </c>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B9" s="16" t="s">
+        <v>256</v>
+      </c>
+      <c r="C9" s="16"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B11" s="4" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B12" s="4" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B13" s="4" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B14" s="4" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B15" s="4" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B16" s="4" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" ht="18" x14ac:dyDescent="0.3">
-      <c r="C17" s="2" t="s">
-        <v>263</v>
-      </c>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B17" s="16" t="s">
+        <v>257</v>
+      </c>
+      <c r="C17" s="16"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" s="4" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" s="4" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B21" s="4" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" s="4" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" s="4" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B24" s="4" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="2:4" ht="18" x14ac:dyDescent="0.3">
@@ -2470,6 +2520,12 @@
       <c r="B37" s="7"/>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2479,196 +2535,201 @@
   <dimension ref="B2:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B11" sqref="B11:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="42.6640625" customWidth="1"/>
-    <col min="3" max="3" width="27.33203125" customWidth="1"/>
+    <col min="3" max="3" width="41.6640625" customWidth="1"/>
     <col min="4" max="4" width="25.109375" customWidth="1"/>
     <col min="5" max="5" width="21.6640625" customWidth="1"/>
-    <col min="6" max="6" width="55.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
-        <v>253</v>
-      </c>
+    <row r="2" spans="2:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="B2" s="15" t="s">
+        <v>247</v>
+      </c>
+      <c r="C2" s="15"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="B11" s="1" t="s">
-        <v>252</v>
-      </c>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="21" x14ac:dyDescent="0.3">
+      <c r="B11" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="C11" s="13"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>67</v>
+        <v>168</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>174</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B14" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B15" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B15" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>181</v>
-      </c>
       <c r="F15" s="4" t="s">
-        <v>182</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B16" s="9" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>75</v>
+        <v>180</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>186</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="9" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>79</v>
+        <v>184</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>190</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B18" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B19" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B19" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>75</v>
-      </c>
       <c r="D19" s="4" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>197</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B11:C11"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>